<commit_message>
feat: design_tools.py and analysis
</commit_message>
<xml_diff>
--- a/PRJ-23/Resultados/Compliance_Matrix.xlsx
+++ b/PRJ-23/Resultados/Compliance_Matrix.xlsx
@@ -226,7 +226,7 @@
     <t>Sim</t>
   </si>
   <si>
-    <t>511355.13 N</t>
+    <t>457055.01 N</t>
   </si>
   <si>
     <t>1800.00 m</t>
@@ -235,22 +235,22 @@
     <t>1150.00 m</t>
   </si>
   <si>
-    <t>10.46 %</t>
-  </si>
-  <si>
-    <t>8.55 %</t>
-  </si>
-  <si>
-    <t>7.49 %</t>
-  </si>
-  <si>
-    <t>13.08 %</t>
-  </si>
-  <si>
-    <t>22.07 %</t>
-  </si>
-  <si>
-    <t>9.34 %</t>
+    <t>6.89 %</t>
+  </si>
+  <si>
+    <t>4.27 %</t>
+  </si>
+  <si>
+    <t>3.70 %</t>
+  </si>
+  <si>
+    <t>9.75 %</t>
+  </si>
+  <si>
+    <t>19.92 %</t>
+  </si>
+  <si>
+    <t>6.78 %</t>
   </si>
   <si>
     <t>0.77</t>
@@ -259,34 +259,34 @@
     <t>36089.24 ft</t>
   </si>
   <si>
-    <t>31514.16 N (Ref T0 req)</t>
-  </si>
-  <si>
-    <t>26.64 %</t>
-  </si>
-  <si>
-    <t>5.46 %</t>
-  </si>
-  <si>
-    <t>-6.78 %</t>
-  </si>
-  <si>
-    <t>-13.18 %</t>
-  </si>
-  <si>
-    <t>-43.55 º</t>
-  </si>
-  <si>
-    <t>7.99 º</t>
-  </si>
-  <si>
-    <t>25.36 º</t>
-  </si>
-  <si>
-    <t>124.65 %</t>
-  </si>
-  <si>
-    <t>34.38 m</t>
+    <t>9106.99 N (Ref T0 req)</t>
+  </si>
+  <si>
+    <t>8.90 %</t>
+  </si>
+  <si>
+    <t>4.54 %</t>
+  </si>
+  <si>
+    <t>9.21 %</t>
+  </si>
+  <si>
+    <t>7.09 %</t>
+  </si>
+  <si>
+    <t>15.76 º</t>
+  </si>
+  <si>
+    <t>19.33 º</t>
+  </si>
+  <si>
+    <t>58.93 º</t>
+  </si>
+  <si>
+    <t>88.97 %</t>
+  </si>
+  <si>
+    <t>30.10 m</t>
   </si>
   <si>
     <t>OK</t>
@@ -921,7 +921,7 @@
         <v>83</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1021,7 +1021,7 @@
         <v>85</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1035,7 +1035,7 @@
         <v>86</v>
       </c>
       <c r="D32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1049,7 +1049,7 @@
         <v>87</v>
       </c>
       <c r="D33" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1077,7 +1077,7 @@
         <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:4">

</xml_diff>